<commit_message>
update file info csv
</commit_message>
<xml_diff>
--- a/Documents/Files_info.xlsx
+++ b/Documents/Files_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lourd\Documents\Data-analytics-bootcamp\Projects\FinalProject\FinalProject\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10D337C9-E216-444F-811C-E90CCC000979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFD10F2-F234-4AA7-A450-A618499D2330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8E62A4BC-C774-4CE8-8DFF-ECC5DF33452D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E62A4BC-C774-4CE8-8DFF-ECC5DF33452D}"/>
   </bookViews>
   <sheets>
     <sheet name="FILES" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="167">
   <si>
     <t>FARS Database (1998-2018)</t>
   </si>
@@ -676,6 +676,18 @@
   <si>
     <t>* Will not be included</t>
   </si>
+  <si>
+    <t>Vehicle number</t>
+  </si>
+  <si>
+    <t>VEH_NO</t>
+  </si>
+  <si>
+    <t>Person type</t>
+  </si>
+  <si>
+    <t>PER_TYP</t>
+  </si>
 </sst>
 </file>
 
@@ -721,7 +733,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -855,24 +867,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -883,10 +892,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -897,19 +925,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -919,13 +934,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1506,11 +1531,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4DE93E-4ECE-4E5A-9DD4-CCB7FAE35A5C}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="18" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="18" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1524,86 +1549,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="I1" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I2" s="4"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="3">
         <v>80</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="3">
         <v>88</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I6" s="8"/>
-      <c r="J6" s="7">
+      <c r="I6" s="23"/>
+      <c r="J6" s="3">
         <v>80</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I9" s="4"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="3:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I14" s="4"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1612,406 +1637,430 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="20"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="10" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
-      <c r="I18" s="10" t="s">
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="I18" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="E19" s="22" t="s">
+      <c r="C19" s="13"/>
+      <c r="E19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="I19" s="22" t="s">
+      <c r="G19" s="14"/>
+      <c r="I19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J19" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="K19" s="16"/>
+      <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="E20" s="21" t="s">
+      <c r="C20" s="13"/>
+      <c r="E20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="I20" s="21" t="s">
+      <c r="G20" s="11"/>
+      <c r="I20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="K20" s="1"/>
+      <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="E21" s="21" t="s">
+      <c r="C21" s="13"/>
+      <c r="E21" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="I21" s="21" t="s">
+      <c r="G21" s="11"/>
+      <c r="I21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="K21" s="1"/>
+      <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="E22" s="21" t="s">
+      <c r="C22" s="13"/>
+      <c r="E22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="I22" s="21" t="s">
+      <c r="G22" s="11"/>
+      <c r="I22" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="K22" s="1"/>
+      <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="E23" s="21" t="s">
+      <c r="C23" s="13"/>
+      <c r="E23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="G23" s="3"/>
-      <c r="I23" s="21" t="s">
+      <c r="G23" s="11"/>
+      <c r="I23" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="K23" s="1"/>
+      <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="E24" s="21" t="s">
+      <c r="C24" s="13"/>
+      <c r="E24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="3"/>
-      <c r="I24" s="21" t="s">
+      <c r="G24" s="11"/>
+      <c r="I24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="K24" s="1"/>
+      <c r="K24" s="10"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="E25" s="21" t="s">
+      <c r="C25" s="13"/>
+      <c r="E25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="I25" s="21" t="s">
+      <c r="G25" s="11"/>
+      <c r="I25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="K25" s="1"/>
+      <c r="K25" s="10"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="E26" s="21" t="s">
+      <c r="C26" s="13"/>
+      <c r="E26" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G26" s="3"/>
-      <c r="I26" s="21" t="s">
+      <c r="G26" s="11"/>
+      <c r="I26" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="K26" s="1"/>
+      <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="E27" s="21" t="s">
+      <c r="C27" s="13"/>
+      <c r="E27" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="I27" s="21" t="s">
+      <c r="G27" s="11"/>
+      <c r="I27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="E28" s="21" t="s">
+      <c r="C28" s="13"/>
+      <c r="E28" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G28" s="3"/>
-      <c r="I28" s="21" t="s">
+      <c r="G28" s="11"/>
+      <c r="I28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="K28" s="1"/>
+      <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="E29" s="21" t="s">
+      <c r="C29" s="13"/>
+      <c r="E29" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="I29" s="21" t="s">
+      <c r="G29" s="11"/>
+      <c r="I29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J29" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="K29" s="1"/>
+      <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="E30" s="21" t="s">
+      <c r="C30" s="13"/>
+      <c r="E30" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="3"/>
-      <c r="I30" s="21" t="s">
+      <c r="G30" s="11"/>
+      <c r="I30" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J30" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="K30" s="1"/>
+      <c r="K30" s="10"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="E31" s="21" t="s">
+      <c r="C31" s="13"/>
+      <c r="E31" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="G31" s="3"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+      <c r="G31" s="11"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="17"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="17"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="17"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="17"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="17"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="17"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="17"/>
+      <c r="C39" s="13"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
+  <mergeCells count="58">
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="F19:G19"/>
@@ -2028,28 +2077,24 @@
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2061,7 +2106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97999C8-8EBA-4595-BF2A-1EF244BFED10}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2085,7 +2130,7 @@
       <c r="B2" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="9" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2181,7 +2226,7 @@
       <c r="A14" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="9" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2245,7 +2290,7 @@
       <c r="A22" t="s">
         <v>143</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="9" t="s">
         <v>144</v>
       </c>
     </row>

</xml_diff>